<commit_message>
Deploying to gh-pages from @ eurovibes/nascontrol-remote@de826c3027ba6282ef51d5a4c04e67440a6fd1b4 🚀
</commit_message>
<xml_diff>
--- a/Fabrication/BoM/nascontrol-remote-bom_0.1.xlsx
+++ b/Fabrication/BoM/nascontrol-remote-bom_0.1.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="91">
   <si>
     <t>Row</t>
   </si>
@@ -59,16 +59,16 @@
     <t>1</t>
   </si>
   <si>
-    <t>C201 C202 C203 C204 C205 C206 C207</t>
+    <t>C101</t>
   </si>
   <si>
     <t>C</t>
   </si>
   <si>
-    <t>100 nF</t>
-  </si>
-  <si>
-    <t>CL05B104KB54PNC</t>
+    <t>1 µF</t>
+  </si>
+  <si>
+    <t>CL31B105KBHNNNE</t>
   </si>
   <si>
     <t>Samsung Electro-Mechanics</t>
@@ -77,243 +77,144 @@
     <t/>
   </si>
   <si>
-    <t>https://jlcpcb.com/partdetail/291005-CL05B104KB54PNC/C307331</t>
-  </si>
-  <si>
-    <t>C_0402_1005Metric</t>
-  </si>
-  <si>
-    <t>50V 100nF X7R ±10% 0402 Multilayer Ceramic Capacitors MLCC - SMD/SMT ROHS</t>
+    <t>https://jlcpcb.com/partdetail/2200-CL31B105KBHNNNE/C1848</t>
+  </si>
+  <si>
+    <t>C_1206_3216Metric</t>
+  </si>
+  <si>
+    <t>50V 1uF X7R ±10% 1206 Multilayer Ceramic Capacitors MLCC - SMD/SMT ROHS</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>H101 H102</t>
+  </si>
+  <si>
+    <t>MountingHole_Pad</t>
+  </si>
+  <si>
+    <t>~</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>MountingHole_3.2mm_M3_Pad</t>
+  </si>
+  <si>
+    <t>Mounting Hole M3</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>J103</t>
+  </si>
+  <si>
+    <t>RJ45_LED_Shielded</t>
+  </si>
+  <si>
+    <t>Control</t>
+  </si>
+  <si>
+    <t>RJHSE-538B</t>
+  </si>
+  <si>
+    <t>Amphenol Communications Solutions</t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/de/details/rjhse538b/rj-steckverbinder/amphenol-communications-solutions/rjhse-538b/</t>
+  </si>
+  <si>
+    <t>RJ45_Amphenol_RJHSE538X</t>
+  </si>
+  <si>
+    <t>Buchse; RJ45; Kat: 5; abgeschirmt,mit LED; System: 8p8c; THT</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>J101 J102 J104</t>
+  </si>
+  <si>
+    <t>Conn_02x05_Odd_Even</t>
+  </si>
+  <si>
+    <t>Serial</t>
+  </si>
+  <si>
+    <t>DS1021-2*5SF11-B</t>
+  </si>
+  <si>
+    <t>CONNFLY</t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/de/details/zl202-10g/stiftleisten-und-buchsen/connfly/ds1021-2-5sf11-b/</t>
+  </si>
+  <si>
+    <t>PinHeader_2x05_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>Stiftleiste; Stift; männlich; PIN: 10; gerade; 2,54mm; THT; 2x5; L3mm</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>R101 R102 R103 R104 R105 R106 R107 R108 R110 R111</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>1 kΩ</t>
+  </si>
+  <si>
+    <t>0402WGF1001TCE</t>
+  </si>
+  <si>
+    <t>UNI-ROYAL(Uniroyal Elec)</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/12256-0402WGF1001TCE/C11702</t>
+  </si>
+  <si>
+    <t>R_0402_1005Metric</t>
+  </si>
+  <si>
+    <t>62.5mW Thick Film Resistors 50V ±100ppm/℃ ±1% -55℃~+155℃ 1kΩ 0402 Chip Resistor - Surface Mount ROHS</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>R109</t>
+  </si>
+  <si>
+    <t>1 MΩ</t>
+  </si>
+  <si>
+    <t>0805W8F1004T5E</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/18202-0805W8F1004T5E/C17514</t>
+  </si>
+  <si>
+    <t>R_0805_2012Metric</t>
+  </si>
+  <si>
+    <t>125mW Thick Film Resistors 150V ±100ppm/℃ ±1% -55℃~+155℃ 1MΩ 0805 Chip Resistor - Surface Mount ROHS</t>
   </si>
   <si>
     <t>7</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>C101</t>
-  </si>
-  <si>
-    <t>1 µF</t>
-  </si>
-  <si>
-    <t>CL31B105KBHNNNE</t>
-  </si>
-  <si>
-    <t>https://jlcpcb.com/partdetail/2200-CL31B105KBHNNNE/C1848</t>
-  </si>
-  <si>
-    <t>C_1206_3216Metric</t>
-  </si>
-  <si>
-    <t>50V 1uF X7R ±10% 1206 Multilayer Ceramic Capacitors MLCC - SMD/SMT ROHS</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>D201</t>
-  </si>
-  <si>
-    <t>NUP2105L</t>
-  </si>
-  <si>
-    <t>NUP2105LT1G</t>
-  </si>
-  <si>
-    <t>TECH PUBLICTECH PUBLIC</t>
-  </si>
-  <si>
-    <t>https://jlcpcb.com/partdetail/TechPublic-NUP2105LT1G/C2890118</t>
-  </si>
-  <si>
-    <t>SOT-23</t>
-  </si>
-  <si>
-    <t>SOT-23 ESD Protection Devices ROHS</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>H101</t>
-  </si>
-  <si>
-    <t>MountingHole</t>
-  </si>
-  <si>
-    <t>~</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>MountingHole_3.2mm_M3</t>
-  </si>
-  <si>
-    <t>Mounting Hole M3</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>H102</t>
-  </si>
-  <si>
-    <t>MountingHole_Pad</t>
-  </si>
-  <si>
-    <t>MountingHole_3.2mm_M3_Pad</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>J103</t>
-  </si>
-  <si>
-    <t>RJ45_LED_Shielded</t>
-  </si>
-  <si>
-    <t>Control</t>
-  </si>
-  <si>
-    <t>RJHSE-538B</t>
-  </si>
-  <si>
-    <t>Amphenol Communications Solutions</t>
-  </si>
-  <si>
-    <t>https://www.tme.eu/de/details/rjhse538b/rj-steckverbinder/amphenol-communications-solutions/rjhse-538b/</t>
-  </si>
-  <si>
-    <t>RJ45_Amphenol_RJHSE538X</t>
-  </si>
-  <si>
-    <t>Buchse; RJ45; Kat: 5; abgeschirmt,mit LED; System: 8p8c; THT</t>
-  </si>
-  <si>
-    <t>J101 J102 J104 J301</t>
-  </si>
-  <si>
-    <t>Conn_02x05_Odd_Even</t>
-  </si>
-  <si>
-    <t>Serial</t>
-  </si>
-  <si>
-    <t>DS1021-2*5SF11-B</t>
-  </si>
-  <si>
-    <t>CONNFLY</t>
-  </si>
-  <si>
-    <t>https://www.tme.eu/de/details/zl202-10g/stiftleisten-und-buchsen/connfly/ds1021-2-5sf11-b/</t>
-  </si>
-  <si>
-    <t>PinHeader_2x05_P2.54mm_Vertical</t>
-  </si>
-  <si>
-    <t>Stiftleiste; Stift; männlich; PIN: 10; gerade; 2,54mm; THT; 2x5; L3mm</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>J302 J303</t>
-  </si>
-  <si>
-    <t>USB_A</t>
-  </si>
-  <si>
-    <t>676430910</t>
-  </si>
-  <si>
-    <t>MOLEX</t>
-  </si>
-  <si>
-    <t>https://www.tme.eu/de/details/mx-67643-0910/usb-und-ieee1394-steckverbinder/molex/676430910/</t>
-  </si>
-  <si>
-    <t>USB_A_Molex_67643_Horizontal</t>
-  </si>
-  <si>
-    <t>Buchse; USB A; auf PCB; THT; PIN: 4; 90°-Winkel; abgeschirmt</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>R201</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>120 Ω</t>
-  </si>
-  <si>
-    <t>1206W4F1200T5E</t>
-  </si>
-  <si>
-    <t>UNI-ROYAL(Uniroyal Elec)</t>
-  </si>
-  <si>
-    <t>https://jlcpcb.com/partdetail/18597-1206W4F1200T5E/C17909</t>
-  </si>
-  <si>
-    <t>R_1206_3216Metric</t>
-  </si>
-  <si>
-    <t>250mW Thick Film Resistors 200V ±100ppm/℃ ±1% -55℃~+155℃ 120Ω 1206 Chip Resistor - Surface Mount ROHS</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>R101 R102 R103 R104 R105 R106 R107 R108 R110 R111</t>
-  </si>
-  <si>
-    <t>1 kΩ</t>
-  </si>
-  <si>
-    <t>0402WGF1001TCE</t>
-  </si>
-  <si>
-    <t>https://jlcpcb.com/partdetail/12256-0402WGF1001TCE/C11702</t>
-  </si>
-  <si>
-    <t>R_0402_1005Metric</t>
-  </si>
-  <si>
-    <t>62.5mW Thick Film Resistors 50V ±100ppm/℃ ±1% -55℃~+155℃ 1kΩ 0402 Chip Resistor - Surface Mount ROHS</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>R109</t>
-  </si>
-  <si>
-    <t>1 MΩ</t>
-  </si>
-  <si>
-    <t>0805W8F1004T5E</t>
-  </si>
-  <si>
-    <t>https://jlcpcb.com/partdetail/18202-0805W8F1004T5E/C17514</t>
-  </si>
-  <si>
-    <t>R_0805_2012Metric</t>
-  </si>
-  <si>
-    <t>125mW Thick Film Resistors 150V ±100ppm/℃ ±1% -55℃~+155℃ 1MΩ 0805 Chip Resistor - Surface Mount ROHS</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
     <t>U101 U102 U103 U104</t>
   </si>
   <si>
@@ -335,78 +236,6 @@
     <t>35V 5000V -55℃~+110℃ 50mA 18us@2mA,100Ω 18us@2mA,100Ω 0.1V@1mA,20mA 1 6V 1.2V Phototransistor DC SMD-4 Optocouplers - Phototransistor Output ROHS</t>
   </si>
   <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>U202</t>
-  </si>
-  <si>
-    <t>ISO3082DW</t>
-  </si>
-  <si>
-    <t>SIT3485ISO</t>
-  </si>
-  <si>
-    <t>SIT</t>
-  </si>
-  <si>
-    <t>https://jlcpcb.com/partdetail/Sit-SIT3485ISO/C2974613</t>
-  </si>
-  <si>
-    <t>SOIC-16W_7.5x10.3mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>SOIC-16 RS-485/RS-422 ICs ROHS</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>U201</t>
-  </si>
-  <si>
-    <t>ICL3232</t>
-  </si>
-  <si>
-    <t>SP3232</t>
-  </si>
-  <si>
-    <t>SP3232EEY-L/TR</t>
-  </si>
-  <si>
-    <t>MaxLinear</t>
-  </si>
-  <si>
-    <t>https://jlcpcb.com/partdetail/Maxlinear-SP3232EEY_LTR/C13482</t>
-  </si>
-  <si>
-    <t>TSSOP-16_4.4x5mm_P0.65mm</t>
-  </si>
-  <si>
-    <t>235Kbps 3V~5.5V transceiver 2/2 TSSOP-16 RS232 ICs ROHS</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>U301 U302</t>
-  </si>
-  <si>
-    <t>USBLC6-2SC6</t>
-  </si>
-  <si>
-    <t>TECH PUBLIC</t>
-  </si>
-  <si>
-    <t>https://jlcpcb.com/partdetail/TechPublic-USBLC62SC6/C2827654</t>
-  </si>
-  <si>
-    <t>SOT-23-6</t>
-  </si>
-  <si>
-    <t>SOT-23-6 ESD Protection Devices ROHS</t>
-  </si>
-  <si>
     <t>KiBot Bill of Materials</t>
   </si>
   <si>
@@ -437,7 +266,7 @@
     <t>KiCad Version:</t>
   </si>
   <si>
-    <t>6.0.5+dfsg-1~bpo11+1</t>
+    <t>7.0.9-7.0.9~ubuntu23.04.1</t>
   </si>
   <si>
     <t>Component Groups:</t>
@@ -605,7 +434,7 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
@@ -614,13 +443,22 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>3641954</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:colOff>3308579</xdr:colOff>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>173152</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="logo.png"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+            <a:ext uri="{C183D7F6-B498-43B3-948B-1728B52AA6E4}">
+              <adec:decorative xmlns:adec="http://schemas.microsoft.com/office/drawing/2017/decorative" val="1"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -931,7 +769,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -943,7 +781,7 @@
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="54.7109375" customWidth="1"/>
     <col min="3" max="3" width="24.7109375" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
     <col min="5" max="5" width="21.7109375" customWidth="1"/>
     <col min="6" max="6" width="38.7109375" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" customWidth="1"/>
@@ -956,7 +794,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>129</v>
+        <v>72</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -970,55 +808,55 @@
     </row>
     <row r="2" spans="1:12">
       <c r="C2" s="2" t="s">
-        <v>130</v>
+        <v>73</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>131</v>
+        <v>74</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>140</v>
+        <v>83</v>
       </c>
       <c r="F2" s="3">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="C3" s="2" t="s">
-        <v>132</v>
+        <v>75</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>133</v>
+        <v>76</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>141</v>
+        <v>84</v>
       </c>
       <c r="F3" s="3">
-        <v>38</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="C4" s="2" t="s">
-        <v>134</v>
+        <v>77</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>135</v>
+        <v>78</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>142</v>
+        <v>85</v>
       </c>
       <c r="F4" s="3">
-        <v>38</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="C5" s="2" t="s">
-        <v>136</v>
+        <v>79</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>137</v>
+        <v>80</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>143</v>
+        <v>86</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1026,16 +864,16 @@
     </row>
     <row r="6" spans="1:12">
       <c r="C6" s="2" t="s">
-        <v>138</v>
+        <v>81</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>139</v>
+        <v>82</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>144</v>
+        <v>87</v>
       </c>
       <c r="F6" s="3">
-        <v>38</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1076,7 +914,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="30.0" customHeight="1">
+    <row r="9" spans="1:12" ht="30" customHeight="1">
       <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
@@ -1111,18 +949,18 @@
         <v>21</v>
       </c>
       <c r="L9" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="8" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="30.0" customHeight="1">
-      <c r="A10" s="8" t="s">
+      <c r="B10" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="C10" s="9" t="s">
         <v>24</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>14</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>25</v>
@@ -1131,7 +969,7 @@
         <v>26</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="G10" s="10" t="s">
         <v>18</v>
@@ -1140,27 +978,27 @@
         <v>18</v>
       </c>
       <c r="I10" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="J10" s="9" t="s">
+      <c r="K10" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="K10" s="10" t="s">
+      <c r="L10" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="30" customHeight="1">
+      <c r="A11" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="L10" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="30.0" customHeight="1">
-      <c r="A11" s="5" t="s">
+      <c r="B11" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="C11" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>32</v>
@@ -1190,7 +1028,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" ht="30" customHeight="1">
       <c r="A12" s="8" t="s">
         <v>38</v>
       </c>
@@ -1207,7 +1045,7 @@
         <v>42</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G12" s="10" t="s">
         <v>18</v>
@@ -1216,36 +1054,36 @@
         <v>18</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="30" customHeight="1">
       <c r="A13" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>18</v>
@@ -1254,37 +1092,37 @@
         <v>18</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="30.0" customHeight="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="30" customHeight="1">
       <c r="A14" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>51</v>
-      </c>
       <c r="D14" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>54</v>
-      </c>
       <c r="G14" s="10" t="s">
         <v>18</v>
       </c>
@@ -1292,36 +1130,36 @@
         <v>18</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="J14" s="9" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="L14" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="30.0" customHeight="1">
+    <row r="15" spans="1:12" ht="45" customHeight="1">
       <c r="A15" s="5" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="G15" s="7" t="s">
         <v>18</v>
@@ -1330,320 +1168,16 @@
         <v>18</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="L15" s="5" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="30.0" customHeight="1">
-      <c r="A16" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="I16" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="J16" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="K16" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="L16" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="30.0" customHeight="1">
-      <c r="A17" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="K17" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="L17" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="30.0" customHeight="1">
-      <c r="A18" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="H18" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="I18" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="J18" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="K18" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="L18" s="8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="30.0" customHeight="1">
-      <c r="A19" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="K19" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="L19" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="45.0" customHeight="1">
-      <c r="A20" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="H20" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="I20" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="J20" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="K20" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="L20" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
-      <c r="A21" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="J21" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="K21" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="L21" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
-      <c r="A22" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="H22" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="I22" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="J22" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="K22" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="L22" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
-      <c r="A23" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H23" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="J23" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="K23" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="L23" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1658,18 +1192,10 @@
     <hyperlink ref="H13" r:id="rId5"/>
     <hyperlink ref="H14" r:id="rId6"/>
     <hyperlink ref="H15" r:id="rId7"/>
-    <hyperlink ref="H16" r:id="rId8"/>
-    <hyperlink ref="H17" r:id="rId9"/>
-    <hyperlink ref="H18" r:id="rId10"/>
-    <hyperlink ref="H19" r:id="rId11"/>
-    <hyperlink ref="H20" r:id="rId12"/>
-    <hyperlink ref="H21" r:id="rId13"/>
-    <hyperlink ref="H22" r:id="rId14"/>
-    <hyperlink ref="H23" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId16"/>
+  <drawing r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -1686,17 +1212,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="6" t="s">
-        <v>145</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>146</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="7" t="s">
-        <v>147</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>